<commit_message>
Results for 30 days and cobb-douglas
</commit_message>
<xml_diff>
--- a/SVM/Results/^ NSEI (3) Metrics Table.xlsx
+++ b/SVM/Results/^ NSEI (3) Metrics Table.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abheesht\Documents\Academics\SOP\Snehanshu\Support Vector Economics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abheesht\Documents\Academics\SOP\Snehanshu\Support-Vector-Economics\SVM\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D1B6D6-B606-478B-A7BB-EFBD04EDC71C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E477C3B4-F4FB-43D2-816F-E22C0B399F04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E7CF4481-218E-4EC8-9CC8-6BD847CFA7F6}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="30">
   <si>
     <t>Linear</t>
   </si>
@@ -116,6 +116,14 @@
   </si>
   <si>
     <t>Average Test Metrics</t>
+  </si>
+  <si>
+    <t>Cobb-Douglas
+Gamma = 0.5</t>
+  </si>
+  <si>
+    <t>Cobb-Douglas
+Gamma = 0.1</t>
   </si>
 </sst>
 </file>
@@ -159,7 +167,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -168,6 +176,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -490,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A29836E0-3C89-4C00-B808-8235CDEF20E1}">
-  <dimension ref="A1:Q23"/>
+  <dimension ref="A1:Q47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,21 +515,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
@@ -529,7 +540,7 @@
       <c r="Q1" s="2"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
+      <c r="A2" s="5"/>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
@@ -565,16 +576,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="1">
-        <v>0.73</v>
+        <v>0.67</v>
       </c>
       <c r="C4" s="1">
-        <v>0.74</v>
+        <v>0.67</v>
       </c>
       <c r="D4" s="1">
-        <v>0.84</v>
+        <v>1</v>
       </c>
       <c r="E4" s="1">
-        <v>0.78</v>
+        <v>0.8</v>
       </c>
       <c r="F4" s="1">
         <v>0.6</v>
@@ -583,10 +594,10 @@
         <v>0.6</v>
       </c>
       <c r="H4" s="1">
-        <v>0.68</v>
+        <v>1</v>
       </c>
       <c r="I4" s="1">
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -598,87 +609,39 @@
       <c r="A6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="1">
-        <v>0.64</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0.67</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0.85</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0.72</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0.53</v>
-      </c>
-      <c r="G6" s="1">
-        <v>0.53</v>
-      </c>
-      <c r="H6" s="1">
-        <v>0.62</v>
-      </c>
-      <c r="I6" s="1">
-        <v>0.55000000000000004</v>
-      </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="1">
-        <v>0.67</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0.66</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0.76</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0.59</v>
-      </c>
-      <c r="G7" s="1">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="H7" s="1">
-        <v>0.85</v>
-      </c>
-      <c r="I7" s="1">
-        <v>0.69</v>
-      </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="1">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="C8" s="1">
         <v>0.66</v>
       </c>
-      <c r="C8" s="1">
-        <v>0.7</v>
-      </c>
       <c r="D8" s="1">
-        <v>0.82</v>
+        <v>0.76</v>
       </c>
       <c r="E8" s="1">
-        <v>0.7</v>
+        <v>0.71</v>
       </c>
       <c r="F8" s="1">
-        <v>0.56999999999999995</v>
+        <v>0.48</v>
       </c>
       <c r="G8" s="1">
-        <v>0.57999999999999996</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="H8" s="1">
-        <v>0.65</v>
+        <v>0.73</v>
       </c>
       <c r="I8" s="1">
-        <v>0.56999999999999995</v>
+        <v>0.63</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -686,28 +649,28 @@
         <v>16</v>
       </c>
       <c r="B9" s="1">
-        <v>0.68</v>
+        <v>0.67</v>
       </c>
       <c r="C9" s="1">
-        <v>0.72</v>
+        <v>0.67</v>
       </c>
       <c r="D9" s="1">
-        <v>0.83</v>
+        <v>1</v>
       </c>
       <c r="E9" s="1">
-        <v>0.73</v>
+        <v>0.8</v>
       </c>
       <c r="F9" s="1">
-        <v>0.59</v>
+        <v>0.6</v>
       </c>
       <c r="G9" s="1">
-        <v>0.56999999999999995</v>
+        <v>0.6</v>
       </c>
       <c r="H9" s="1">
-        <v>0.73</v>
+        <v>1</v>
       </c>
       <c r="I9" s="1">
-        <v>0.61</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -715,28 +678,28 @@
         <v>15</v>
       </c>
       <c r="B10" s="1">
-        <v>0.68</v>
+        <v>0.67</v>
       </c>
       <c r="C10" s="1">
-        <v>0.73</v>
+        <v>0.67</v>
       </c>
       <c r="D10" s="1">
-        <v>0.82</v>
+        <v>1</v>
       </c>
       <c r="E10" s="1">
-        <v>0.72</v>
+        <v>0.8</v>
       </c>
       <c r="F10" s="1">
-        <v>0.56000000000000005</v>
+        <v>0.6</v>
       </c>
       <c r="G10" s="1">
-        <v>0.53</v>
+        <v>0.6</v>
       </c>
       <c r="H10" s="1">
-        <v>0.62</v>
+        <v>1</v>
       </c>
       <c r="I10" s="1">
-        <v>0.54</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -744,28 +707,28 @@
         <v>14</v>
       </c>
       <c r="B11" s="1">
-        <v>0.7</v>
+        <v>0.67</v>
       </c>
       <c r="C11" s="1">
-        <v>0.74</v>
+        <v>0.67</v>
       </c>
       <c r="D11" s="1">
-        <v>0.84</v>
+        <v>1</v>
       </c>
       <c r="E11" s="1">
-        <v>0.74</v>
+        <v>0.8</v>
       </c>
       <c r="F11" s="1">
-        <v>0.61</v>
+        <v>0.6</v>
       </c>
       <c r="G11" s="1">
-        <v>0.56999999999999995</v>
+        <v>0.6</v>
       </c>
       <c r="H11" s="1">
-        <v>0.73</v>
+        <v>1</v>
       </c>
       <c r="I11" s="1">
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -773,28 +736,28 @@
         <v>13</v>
       </c>
       <c r="B12" s="1">
-        <v>0.7</v>
+        <v>0.67</v>
       </c>
       <c r="C12" s="1">
-        <v>0.74</v>
+        <v>0.67</v>
       </c>
       <c r="D12" s="1">
-        <v>0.84</v>
+        <v>1</v>
       </c>
       <c r="E12" s="1">
-        <v>0.74</v>
+        <v>0.8</v>
       </c>
       <c r="F12" s="1">
-        <v>0.56999999999999995</v>
+        <v>0.6</v>
       </c>
       <c r="G12" s="1">
-        <v>0.59</v>
+        <v>0.6</v>
       </c>
       <c r="H12" s="1">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="I12" s="1">
-        <v>0.55000000000000004</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -802,28 +765,28 @@
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>0.71</v>
+        <v>0.67</v>
       </c>
       <c r="C13" s="1">
-        <v>0.76</v>
+        <v>0.67</v>
       </c>
       <c r="D13" s="1">
-        <v>0.84</v>
+        <v>1</v>
       </c>
       <c r="E13" s="1">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="F13" s="1">
-        <v>0.57999999999999996</v>
+        <v>0.6</v>
       </c>
       <c r="G13" s="1">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="H13" s="1">
-        <v>0.69</v>
+        <v>1</v>
       </c>
       <c r="I13" s="1">
-        <v>0.56000000000000005</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -831,28 +794,28 @@
         <v>11</v>
       </c>
       <c r="B14" s="1">
-        <v>0.71</v>
+        <v>0.67</v>
       </c>
       <c r="C14" s="1">
-        <v>0.77</v>
+        <v>0.67</v>
       </c>
       <c r="D14" s="1">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="E14" s="1">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="F14" s="1">
-        <v>0.56999999999999995</v>
+        <v>0.6</v>
       </c>
       <c r="G14" s="1">
-        <v>0.56999999999999995</v>
+        <v>0.6</v>
       </c>
       <c r="H14" s="1">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="I14" s="1">
-        <v>0.55000000000000004</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -860,28 +823,28 @@
         <v>10</v>
       </c>
       <c r="B15" s="1">
-        <v>0.73</v>
+        <v>0.67</v>
       </c>
       <c r="C15" s="1">
-        <v>0.78</v>
+        <v>0.67</v>
       </c>
       <c r="D15" s="1">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="E15" s="1">
-        <v>0.77</v>
+        <v>0.8</v>
       </c>
       <c r="F15" s="1">
-        <v>0.57999999999999996</v>
+        <v>0.6</v>
       </c>
       <c r="G15" s="1">
-        <v>0.53</v>
+        <v>0.6</v>
       </c>
       <c r="H15" s="1">
-        <v>0.67</v>
+        <v>1</v>
       </c>
       <c r="I15" s="1">
-        <v>0.56000000000000005</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
@@ -889,28 +852,28 @@
         <v>9</v>
       </c>
       <c r="B16" s="1">
-        <v>0.73</v>
+        <v>0.67</v>
       </c>
       <c r="C16" s="1">
-        <v>0.78</v>
+        <v>0.67</v>
       </c>
       <c r="D16" s="1">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="E16" s="1">
-        <v>0.77</v>
+        <v>0.8</v>
       </c>
       <c r="F16" s="1">
-        <v>0.55000000000000004</v>
+        <v>0.6</v>
       </c>
       <c r="G16" s="1">
-        <v>0.54</v>
+        <v>0.6</v>
       </c>
       <c r="H16" s="1">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="I16" s="1">
-        <v>0.54</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -923,28 +886,28 @@
         <v>24</v>
       </c>
       <c r="B18" s="1">
-        <v>0.59</v>
+        <v>0.67</v>
       </c>
       <c r="C18" s="1">
-        <v>0.59</v>
+        <v>0.67</v>
       </c>
       <c r="D18" s="1">
         <v>1</v>
       </c>
       <c r="E18" s="1">
-        <v>0.74</v>
+        <v>0.8</v>
       </c>
       <c r="F18" s="1">
-        <v>0.56999999999999995</v>
+        <v>0.6</v>
       </c>
       <c r="G18" s="1">
-        <v>0.56999999999999995</v>
+        <v>0.6</v>
       </c>
       <c r="H18" s="1">
         <v>1</v>
       </c>
       <c r="I18" s="1">
-        <v>0.72</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -952,28 +915,28 @@
         <v>23</v>
       </c>
       <c r="B19" s="1">
-        <v>0.59</v>
+        <v>0.67</v>
       </c>
       <c r="C19" s="1">
-        <v>0.59</v>
+        <v>0.67</v>
       </c>
       <c r="D19" s="1">
         <v>1</v>
       </c>
       <c r="E19" s="1">
-        <v>0.74</v>
+        <v>0.8</v>
       </c>
       <c r="F19" s="1">
-        <v>0.56999999999999995</v>
+        <v>0.6</v>
       </c>
       <c r="G19" s="1">
-        <v>0.56999999999999995</v>
+        <v>0.6</v>
       </c>
       <c r="H19" s="1">
         <v>1</v>
       </c>
       <c r="I19" s="1">
-        <v>0.72</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -981,28 +944,28 @@
         <v>22</v>
       </c>
       <c r="B20" s="1">
-        <v>0.59</v>
+        <v>0.67</v>
       </c>
       <c r="C20" s="1">
-        <v>0.59</v>
+        <v>0.67</v>
       </c>
       <c r="D20" s="1">
         <v>1</v>
       </c>
       <c r="E20" s="1">
-        <v>0.74</v>
+        <v>0.8</v>
       </c>
       <c r="F20" s="1">
-        <v>0.56999999999999995</v>
+        <v>0.6</v>
       </c>
       <c r="G20" s="1">
-        <v>0.56999999999999995</v>
+        <v>0.6</v>
       </c>
       <c r="H20" s="1">
         <v>1</v>
       </c>
       <c r="I20" s="1">
-        <v>0.72</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1010,28 +973,28 @@
         <v>21</v>
       </c>
       <c r="B21" s="1">
-        <v>0.59</v>
+        <v>0.67</v>
       </c>
       <c r="C21" s="1">
-        <v>0.59</v>
+        <v>0.67</v>
       </c>
       <c r="D21" s="1">
         <v>1</v>
       </c>
       <c r="E21" s="1">
-        <v>0.74</v>
+        <v>0.8</v>
       </c>
       <c r="F21" s="1">
-        <v>0.56999999999999995</v>
+        <v>0.6</v>
       </c>
       <c r="G21" s="1">
-        <v>0.56999999999999995</v>
+        <v>0.6</v>
       </c>
       <c r="H21" s="1">
         <v>1</v>
       </c>
       <c r="I21" s="1">
-        <v>0.72</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1039,28 +1002,28 @@
         <v>20</v>
       </c>
       <c r="B22" s="1">
-        <v>0.59</v>
+        <v>0.67</v>
       </c>
       <c r="C22" s="1">
-        <v>0.59</v>
+        <v>0.67</v>
       </c>
       <c r="D22" s="1">
         <v>1</v>
       </c>
       <c r="E22" s="1">
-        <v>0.74</v>
+        <v>0.8</v>
       </c>
       <c r="F22" s="1">
-        <v>0.56999999999999995</v>
+        <v>0.6</v>
       </c>
       <c r="G22" s="1">
-        <v>0.56999999999999995</v>
+        <v>0.6</v>
       </c>
       <c r="H22" s="1">
         <v>1</v>
       </c>
       <c r="I22" s="1">
-        <v>0.72</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1068,28 +1031,532 @@
         <v>19</v>
       </c>
       <c r="B23" s="1">
-        <v>0.59</v>
+        <v>0.67</v>
       </c>
       <c r="C23" s="1">
-        <v>0.59</v>
+        <v>0.67</v>
       </c>
       <c r="D23" s="1">
         <v>1</v>
       </c>
       <c r="E23" s="1">
-        <v>0.74</v>
+        <v>0.8</v>
       </c>
       <c r="F23" s="1">
-        <v>0.56999999999999995</v>
+        <v>0.6</v>
       </c>
       <c r="G23" s="1">
-        <v>0.56999999999999995</v>
+        <v>0.6</v>
       </c>
       <c r="H23" s="1">
         <v>1</v>
       </c>
       <c r="I23" s="1">
-        <v>0.72</v>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="G28" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="H28" s="1">
+        <v>1</v>
+      </c>
+      <c r="I28" s="1">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1</v>
+      </c>
+      <c r="E29" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="F29" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="G29" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="H29" s="1">
+        <v>1</v>
+      </c>
+      <c r="I29" s="1">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="D30" s="1">
+        <v>1</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="F30" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="G30" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="H30" s="1">
+        <v>1</v>
+      </c>
+      <c r="I30" s="1">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="F31" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="G31" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="H31" s="1">
+        <v>1</v>
+      </c>
+      <c r="I31" s="1">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="C32" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="D32" s="1">
+        <v>1</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="F32" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="G32" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="H32" s="1">
+        <v>1</v>
+      </c>
+      <c r="I32" s="1">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="F33" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="G33" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="H33" s="1">
+        <v>1</v>
+      </c>
+      <c r="I33" s="1">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="C34" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="D34" s="1">
+        <v>1</v>
+      </c>
+      <c r="E34" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="F34" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="G34" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="H34" s="1">
+        <v>1</v>
+      </c>
+      <c r="I34" s="1">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="C35" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="D35" s="1">
+        <v>1</v>
+      </c>
+      <c r="E35" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="F35" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="G35" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="H35" s="1">
+        <v>1</v>
+      </c>
+      <c r="I35" s="1">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B40" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="C40" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="D40" s="1">
+        <v>1</v>
+      </c>
+      <c r="E40" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="F40" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="G40" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="H40" s="1">
+        <v>1</v>
+      </c>
+      <c r="I40" s="1">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B41" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="C41" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="D41" s="1">
+        <v>1</v>
+      </c>
+      <c r="E41" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="F41" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="G41" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="H41" s="1">
+        <v>1</v>
+      </c>
+      <c r="I41" s="1">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="C42" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="D42" s="1">
+        <v>1</v>
+      </c>
+      <c r="E42" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="F42" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="G42" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="H42" s="1">
+        <v>1</v>
+      </c>
+      <c r="I42" s="1">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B43" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="C43" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="D43" s="1">
+        <v>1</v>
+      </c>
+      <c r="E43" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="F43" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="G43" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="H43" s="1">
+        <v>1</v>
+      </c>
+      <c r="I43" s="1">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="C44" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="D44" s="1">
+        <v>1</v>
+      </c>
+      <c r="E44" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="F44" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="G44" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="H44" s="1">
+        <v>1</v>
+      </c>
+      <c r="I44" s="1">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B45" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="C45" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="D45" s="1">
+        <v>1</v>
+      </c>
+      <c r="E45" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="F45" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="G45" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="H45" s="1">
+        <v>1</v>
+      </c>
+      <c r="I45" s="1">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B46" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="C46" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="D46" s="1">
+        <v>1</v>
+      </c>
+      <c r="E46" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="F46" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="G46" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="H46" s="1">
+        <v>1</v>
+      </c>
+      <c r="I46" s="1">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B47" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="C47" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="D47" s="1">
+        <v>1</v>
+      </c>
+      <c r="E47" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="F47" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="G47" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="H47" s="1">
+        <v>1</v>
+      </c>
+      <c r="I47" s="1">
+        <v>0.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>